<commit_message>
fix the third zone impedance calculation
</commit_message>
<xml_diff>
--- a/protection_zones.xlsx
+++ b/protection_zones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587FAB96-E3AB-41A0-A378-AB82C6DDDEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF6C50-5511-46D4-ABF4-86B23BB76FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="check_sheet" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
     <t>1.1687375+9.100861j</t>
   </si>
   <si>
-    <t>(2.4147786375+18.803678949j)</t>
-  </si>
-  <si>
     <t>(2.022583725+15.749690022j)</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>1.11864875+8.7108241j</t>
   </si>
   <si>
-    <t>(2.22799768875+17.3492313489j)</t>
-  </si>
-  <si>
     <t>(1.8077029875+14.076431721j)</t>
   </si>
   <si>
@@ -236,6 +230,12 @@
   </si>
   <si>
     <t>(2.8385294625000004+22.103391122999998j)</t>
+  </si>
+  <si>
+    <t>(1.7167919062499999+13.368514747499999j)</t>
+  </si>
+  <si>
+    <t>(2.04963165+15.960309947999999j)</t>
   </si>
 </sst>
 </file>
@@ -257,6 +257,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -267,18 +268,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -317,21 +312,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,24 +631,24 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,13 +670,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -699,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H2" t="str">
         <f>IMPRODUCT(B27,0.9)</f>
@@ -709,12 +703,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B37),IMPRODUCT(0.9,B27))</f>
         <v>1.41250275+10.99904058j</v>
       </c>
-      <c r="J2" t="str">
-        <f>IMSUM(IMPRODUCT(0.729,B39),IMPRODUCT(0.81,B37),IMPRODUCT(0.9,B27))</f>
-        <v>2.22799768875+17.3492313489j</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="6" t="str">
+        <f>IMSUM(IMPRODUCT(0.729*0.5,B25),IMPRODUCT(0.81,B37),IMPRODUCT(0.9,B27))</f>
+        <v>1.71679190625+13.3685147475j</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -746,7 +740,7 @@
         <v>1.65292875+12.8712177j</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -763,7 +757,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H4" t="str">
         <f>IMPRODUCT(B25,0.9)</f>
@@ -773,12 +767,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B25))</f>
         <v>1.562769+12.16915128j</v>
       </c>
-      <c r="J4" s="7" t="str">
+      <c r="J4" s="6" t="str">
         <f>IMSUM(IMPRODUCT(0.729,B27),IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B25))</f>
         <v>2.04963165+15.960309948j</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -795,7 +789,7 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" t="str">
         <f>IMPRODUCT(B25,0.9)</f>
@@ -810,7 +804,7 @@
         <v>2.022583725+15.749690022j</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -827,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H6" t="str">
         <f>IMPRODUCT(B26,0.9)</f>
@@ -837,12 +831,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B26))</f>
         <v>1.562769+12.16915128j</v>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="6" t="str">
         <f>IMSUM(IMPRODUCT(0.729,B27),IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B26))</f>
         <v>2.04963165+15.960309948j</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -859,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" t="str">
         <f>IMPRODUCT(B26,0.9)</f>
@@ -874,7 +868,7 @@
         <v>2.022583725+15.749690022j</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -906,7 +900,7 @@
         <v>2.38756375+18.5917589j</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -938,7 +932,7 @@
         <v>2.04737765625+15.9427582875j</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -970,7 +964,7 @@
         <v>2.16759065625+16.8788468475j</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1002,7 +996,7 @@
         <v>1.89711140625+14.7726475875j</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1034,7 +1028,7 @@
         <v>2.02024625+15.7314883j</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1051,7 +1045,7 @@
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" t="str">
         <f>IMPRODUCT(B30,0.9)</f>
@@ -1066,7 +1060,7 @@
         <v>2.335137525+18.183520278j</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1080,10 +1074,10 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H14" t="str">
         <f>IMPRODUCT(B37,0.9)</f>
@@ -1098,7 +1092,7 @@
         <v>2.7814282875+21.658749057j</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1130,7 +1124,7 @@
         <v>1.74684515625+13.6025368875j</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1144,28 +1138,28 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" t="s">
-        <v>61</v>
       </c>
       <c r="H16" t="str">
         <f>IMPRODUCT(B39,0.9)</f>
         <v>1.006783875+7.83974169j</v>
       </c>
-      <c r="I16" s="7" t="str">
-        <f>IMSUM(IMPRODUCT(0.81,B28),IMPRODUCT(0.9,B38))</f>
-        <v>2.13378075+16.61557194j</v>
+      <c r="I16" s="6" t="str">
+        <f>IMSUM(IMPRODUCT(0.81,B28),IMPRODUCT(0.9,B39))</f>
+        <v>2.088700875+16.26453873j</v>
       </c>
       <c r="J16" t="str">
         <f>IMSUM(IMPRODUCT(0.729*0.5,B25),IMPRODUCT(0.81,B28),IMPRODUCT(0.9,B39))</f>
         <v>2.39299003125+18.6340128975j</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1179,13 +1173,13 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H17" t="str">
         <f>IMPRODUCT(B39,0.9)</f>
@@ -1200,7 +1194,7 @@
         <v>2.305084275+17.949498138j</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1232,7 +1226,7 @@
         <v>2.38756375+18.5917589j</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1246,10 +1240,10 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19" t="str">
         <f>IMPRODUCT(B28,0.9)</f>
@@ -1264,129 +1258,129 @@
         <v>2.8385294625+22.103391123j</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>12</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>13</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>14</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>55</v>
+      <c r="B39" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1409,18 +1403,18 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.765625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -1458,627 +1452,627 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>25</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="3">
         <v>1.5</v>
       </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="str">
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="str">
         <f>IMPRODUCT(COMPLEX(E2, F2, "j"), D2)</f>
         <v>0.8348125+6.500615j</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>25</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <v>1.5</v>
       </c>
-      <c r="L3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6" t="str">
-        <f t="shared" ref="N3:N16" si="0">IMPRODUCT(COMPLEX(E3, F3, "j"), D3)</f>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N15" si="0">IMPRODUCT(COMPLEX(E3, F3, "j"), D3)</f>
         <v>0.8348125+6.500615j</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>20</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>1.5</v>
       </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6" t="str">
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" t="str">
         <f t="shared" si="0"/>
         <v>0.66785+5.200492j</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>40</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>1.5</v>
       </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6" t="str">
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="0"/>
         <v>1.3357+10.400984j</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>40</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>1.5</v>
       </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6" t="str">
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="0"/>
         <v>1.3357+10.400984j</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>30</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="3">
         <v>1.5</v>
       </c>
-      <c r="L7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6" t="str">
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="0"/>
         <v>1.001775+7.800738j</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>1.5</v>
       </c>
-      <c r="L8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6" t="str">
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="0"/>
         <v>0.13357+1.0400984j</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>15</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="3">
         <v>1.5</v>
       </c>
-      <c r="L9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6" t="str">
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="0"/>
         <v>0.5008875+3.900369j</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="2">
         <v>7</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>0.5</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="3">
         <v>1.5</v>
       </c>
-      <c r="L10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6" t="str">
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="0"/>
         <v>0.01669625+0.1300123j</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="3">
         <v>1.5</v>
       </c>
-      <c r="L11" s="4">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6" t="str">
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="0"/>
         <v>0.1669625+1.300123j</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>10</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>4</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="3">
         <v>1.5</v>
       </c>
-      <c r="L12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6" t="str">
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" t="str">
         <f t="shared" si="0"/>
         <v>0.13357+1.0400984j</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="3">
         <v>1.5</v>
       </c>
-      <c r="L13" s="4">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6" t="str">
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" t="str">
         <f t="shared" si="0"/>
         <v>0.1669625+1.300123j</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>3</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>4</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>30</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="3">
         <v>1.5</v>
       </c>
-      <c r="L14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6" t="str">
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" t="str">
         <f t="shared" si="0"/>
         <v>1.001775+7.800738j</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>4</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <v>35</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="3">
         <v>1.5</v>
       </c>
-      <c r="L15" s="4">
-        <v>1</v>
-      </c>
-      <c r="N15" s="6" t="str">
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" t="str">
         <f t="shared" si="0"/>
         <v>1.1687375+9.100861j</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <f>SUM(D8:D13)</f>
         <v>33.5</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>3.3392499999999999E-2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <v>0.26002459999999999</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="3">
         <v>1.365E-8</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="3">
         <v>0.11815589999999999</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="3">
         <v>0.97861880000000001</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="3">
         <v>5.4800000000000001E-9</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="3">
         <v>1.5</v>
       </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="N16" s="6" t="str">
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" t="str">
         <f>IMPRODUCT(COMPLEX(E16, F16, "j"), D16)</f>
         <v>1.11864875+8.7108241j</v>
       </c>

</xml_diff>

<commit_message>
Parallel line delete test and negative direction, round the measurement
compared with last version, the parellel line is deleted, so around 1000 faults detection is spared.
</commit_message>
<xml_diff>
--- a/protection_zones.xlsx
+++ b/protection_zones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF6C50-5511-46D4-ABF4-86B23BB76FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C414E9-3FD3-4D1A-9DEE-BF57216FC37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="check_sheet" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -325,7 +325,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,24 +630,24 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.53515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.23046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +675,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -703,12 +702,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B37),IMPRODUCT(0.9,B27))</f>
         <v>1.41250275+10.99904058j</v>
       </c>
-      <c r="J2" s="6" t="str">
+      <c r="J2" t="str">
         <f>IMSUM(IMPRODUCT(0.729*0.5,B25),IMPRODUCT(0.81,B37),IMPRODUCT(0.9,B27))</f>
         <v>1.71679190625+13.3685147475j</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -740,7 +739,7 @@
         <v>1.65292875+12.8712177j</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -767,12 +766,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B25))</f>
         <v>1.562769+12.16915128j</v>
       </c>
-      <c r="J4" s="6" t="str">
+      <c r="J4" t="str">
         <f>IMSUM(IMPRODUCT(0.729,B27),IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B25))</f>
         <v>2.04963165+15.960309948j</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -804,7 +803,7 @@
         <v>2.022583725+15.749690022j</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -831,12 +830,12 @@
         <f>IMSUM(IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B26))</f>
         <v>1.562769+12.16915128j</v>
       </c>
-      <c r="J6" s="6" t="str">
+      <c r="J6" t="str">
         <f>IMSUM(IMPRODUCT(0.729,B27),IMPRODUCT(0.81,B30),IMPRODUCT(0.9,B26))</f>
         <v>2.04963165+15.960309948j</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -868,7 +867,7 @@
         <v>2.022583725+15.749690022j</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -900,7 +899,7 @@
         <v>2.38756375+18.5917589j</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -932,7 +931,7 @@
         <v>2.04737765625+15.9427582875j</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -964,7 +963,7 @@
         <v>2.16759065625+16.8788468475j</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -996,7 +995,7 @@
         <v>1.89711140625+14.7726475875j</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1028,7 +1027,7 @@
         <v>2.02024625+15.7314883j</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>2.335137525+18.183520278j</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1092,7 +1091,7 @@
         <v>2.7814282875+21.658749057j</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>1.74684515625+13.6025368875j</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1150,7 +1149,7 @@
         <f>IMPRODUCT(B39,0.9)</f>
         <v>1.006783875+7.83974169j</v>
       </c>
-      <c r="I16" s="6" t="str">
+      <c r="I16" t="str">
         <f>IMSUM(IMPRODUCT(0.81,B28),IMPRODUCT(0.9,B39))</f>
         <v>2.088700875+16.26453873j</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>2.39299003125+18.6340128975j</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>2.305084275+17.949498138j</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1226,7 +1225,7 @@
         <v>2.38756375+18.5917589j</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1258,12 +1257,12 @@
         <v>2.8385294625+22.103391123j</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1303,7 +1302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>13</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>14</v>
       </c>
@@ -1403,18 +1402,18 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.53515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>0.8348125+6.500615j</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>0.8348125+6.500615j</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>0.66785+5.200492j</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1.3357+10.400984j</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1662,7 +1661,7 @@
         <v>1.3357+10.400984j</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>1.001775+7.800738j</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>0.13357+1.0400984j</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>0.5008875+3.900369j</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>0.01669625+0.1300123j</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>0.1669625+1.300123j</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>0.13357+1.0400984j</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>0.1669625+1.300123j</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>1.001775+7.800738j</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>1.1687375+9.100861j</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>